<commit_message>
Cross-matched through World Traveler
</commit_message>
<xml_diff>
--- a/data_2017_5_9/imdb/imdb_matches_wf.xlsx
+++ b/data_2017_5_9/imdb/imdb_matches_wf.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2641" uniqueCount="1485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="1504">
   <si>
     <t>mauvais99ions</t>
   </si>
@@ -4750,6 +4750,63 @@
   </si>
   <si>
     <t>key</t>
+  </si>
+  <si>
+    <t>badmara99bord</t>
+  </si>
+  <si>
+    <t>Bad ma ra khahad bord (1999)</t>
+  </si>
+  <si>
+    <t>Bad ma ra khahad bord</t>
+  </si>
+  <si>
+    <t>winters97afer</t>
+  </si>
+  <si>
+    <t>Winterschläfer (1997)</t>
+  </si>
+  <si>
+    <t>Winterschläfer</t>
+  </si>
+  <si>
+    <t>wisdom98iles</t>
+  </si>
+  <si>
+    <t>The Wisdom of Crocodiles (1998)</t>
+  </si>
+  <si>
+    <t>The Wisdom of Crocodiles</t>
+  </si>
+  <si>
+    <t>wolveso98omer</t>
+  </si>
+  <si>
+    <t>The Wolves of Kromer (1998)</t>
+  </si>
+  <si>
+    <t>The Wolves of Kromer</t>
+  </si>
+  <si>
+    <t>womanch99aser</t>
+  </si>
+  <si>
+    <t>The Woman Chaser (1999)</t>
+  </si>
+  <si>
+    <t>The Woman Chaser</t>
+  </si>
+  <si>
+    <t>0000011212</t>
+  </si>
+  <si>
+    <t>wonderl99land</t>
+  </si>
+  <si>
+    <t>Wonderland (1999)</t>
+  </si>
+  <si>
+    <t>Wonderland</t>
   </si>
 </sst>
 </file>
@@ -5148,9 +5205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS328"/>
+  <dimension ref="A1:AT334"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
+      <selection activeCell="A334" sqref="A334"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -44119,15 +44178,15 @@
         <v>0</v>
       </c>
       <c r="AP281" t="str">
-        <f t="shared" ref="AP281:AP328" si="20">IF(LEFT(D281,2)="A",MID(D281,3,9999),D281)</f>
+        <f t="shared" ref="AP281:AP334" si="20">IF(LEFT(D281,2)="A",MID(D281,3,9999),D281)</f>
         <v>Swiri</v>
       </c>
       <c r="AQ281" t="str">
-        <f t="shared" ref="AQ281:AQ328" si="21">IF(LEFT(AP281,4)="The ",MID(AP281,5,9999),AP281)</f>
+        <f t="shared" ref="AQ281:AQ334" si="21">IF(LEFT(AP281,4)="The ",MID(AP281,5,9999),AP281)</f>
         <v>Swiri</v>
       </c>
       <c r="AR281" t="str">
-        <f t="shared" ref="AR281:AR328" si="22">LOWER(CONCATENATE(LEFT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),7),RIGHT(F281,2),RIGHT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),4)))</f>
+        <f t="shared" ref="AR281:AR334" si="22">LOWER(CONCATENATE(LEFT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),7),RIGHT(F281,2),RIGHT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),4)))</f>
         <v>swiri99wiri</v>
       </c>
       <c r="AS281" t="str">
@@ -49571,7 +49630,7 @@
         <v>vénusbe99tut]</v>
       </c>
     </row>
-    <row r="321" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>1456</v>
       </c>
@@ -49712,7 +49771,7 @@
         <v>virgins99ides</v>
       </c>
     </row>
-    <row r="322" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>1459</v>
       </c>
@@ -49853,7 +49912,7 @@
         <v>wadd:th99lmes</v>
       </c>
     </row>
-    <row r="323" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>1462</v>
       </c>
@@ -49991,7 +50050,7 @@
         <v>wagajin93toki</v>
       </c>
     </row>
-    <row r="324" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>1465</v>
       </c>
@@ -50132,7 +50191,7 @@
         <v>awakein99ence</v>
       </c>
     </row>
-    <row r="325" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>1468</v>
       </c>
@@ -50270,7 +50329,7 @@
         <v>weekend99kend</v>
       </c>
     </row>
-    <row r="326" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>1472</v>
       </c>
@@ -50411,7 +50470,7 @@
         <v>wenttoc98five</v>
       </c>
     </row>
-    <row r="327" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>1476</v>
       </c>
@@ -50552,7 +50611,7 @@
         <v>whateve99ith?</v>
       </c>
     </row>
-    <row r="328" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>1479</v>
       </c>
@@ -50691,6 +50750,858 @@
       <c r="AS328" t="str">
         <f t="shared" si="23"/>
         <v>wildflo99wers</v>
+      </c>
+    </row>
+    <row r="329" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B329">
+        <v>177701</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D329" s="4" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E329" s="4" t="s">
+        <v>1487</v>
+      </c>
+      <c r="F329" s="4">
+        <v>1999</v>
+      </c>
+      <c r="G329">
+        <v>1999</v>
+      </c>
+      <c r="H329">
+        <v>7.6</v>
+      </c>
+      <c r="I329">
+        <v>118</v>
+      </c>
+      <c r="J329">
+        <v>5918</v>
+      </c>
+      <c r="K329" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="L329">
+        <v>-1</v>
+      </c>
+      <c r="M329">
+        <v>213253</v>
+      </c>
+      <c r="N329" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="O329" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q329">
+        <v>0</v>
+      </c>
+      <c r="R329">
+        <v>0</v>
+      </c>
+      <c r="S329">
+        <v>0</v>
+      </c>
+      <c r="T329">
+        <v>0</v>
+      </c>
+      <c r="U329">
+        <v>0</v>
+      </c>
+      <c r="V329">
+        <v>0</v>
+      </c>
+      <c r="W329">
+        <v>0</v>
+      </c>
+      <c r="X329">
+        <v>0</v>
+      </c>
+      <c r="Y329">
+        <v>1</v>
+      </c>
+      <c r="Z329">
+        <v>0</v>
+      </c>
+      <c r="AA329">
+        <v>0</v>
+      </c>
+      <c r="AB329">
+        <v>0</v>
+      </c>
+      <c r="AC329">
+        <v>0</v>
+      </c>
+      <c r="AD329">
+        <v>0</v>
+      </c>
+      <c r="AE329">
+        <v>0</v>
+      </c>
+      <c r="AF329">
+        <v>0</v>
+      </c>
+      <c r="AG329">
+        <v>0</v>
+      </c>
+      <c r="AH329">
+        <v>0</v>
+      </c>
+      <c r="AI329">
+        <v>0</v>
+      </c>
+      <c r="AJ329">
+        <v>0</v>
+      </c>
+      <c r="AK329">
+        <v>0</v>
+      </c>
+      <c r="AL329">
+        <v>0</v>
+      </c>
+      <c r="AM329">
+        <v>0</v>
+      </c>
+      <c r="AN329">
+        <v>0</v>
+      </c>
+      <c r="AO329">
+        <v>0</v>
+      </c>
+      <c r="AP329" t="str">
+        <f t="shared" si="20"/>
+        <v>Bad ma ra khahad bord</v>
+      </c>
+      <c r="AQ329" t="str">
+        <f t="shared" si="21"/>
+        <v>Bad ma ra khahad bord</v>
+      </c>
+      <c r="AR329" t="str">
+        <f t="shared" si="22"/>
+        <v>badmara99bord</v>
+      </c>
+      <c r="AS329" t="s">
+        <v>1485</v>
+      </c>
+      <c r="AT329" t="str">
+        <f t="shared" ref="AT329:AT334" si="24">IF(ISBLANK(AS329),AR329,AS329)</f>
+        <v>badmara99bord</v>
+      </c>
+    </row>
+    <row r="330" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B330">
+        <v>353254</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D330" s="4" t="s">
+        <v>1490</v>
+      </c>
+      <c r="E330" s="4" t="s">
+        <v>1490</v>
+      </c>
+      <c r="F330" s="4">
+        <v>1997</v>
+      </c>
+      <c r="G330">
+        <v>1997</v>
+      </c>
+      <c r="H330">
+        <v>7.3</v>
+      </c>
+      <c r="I330">
+        <v>122</v>
+      </c>
+      <c r="J330">
+        <v>3976</v>
+      </c>
+      <c r="K330" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="L330">
+        <v>-1</v>
+      </c>
+      <c r="M330">
+        <v>316431</v>
+      </c>
+      <c r="N330" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="O330" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="Q330">
+        <v>0</v>
+      </c>
+      <c r="R330">
+        <v>0</v>
+      </c>
+      <c r="S330">
+        <v>0</v>
+      </c>
+      <c r="T330">
+        <v>0</v>
+      </c>
+      <c r="U330">
+        <v>0</v>
+      </c>
+      <c r="V330">
+        <v>0</v>
+      </c>
+      <c r="W330">
+        <v>0</v>
+      </c>
+      <c r="X330">
+        <v>0</v>
+      </c>
+      <c r="Y330">
+        <v>1</v>
+      </c>
+      <c r="Z330">
+        <v>0</v>
+      </c>
+      <c r="AA330">
+        <v>0</v>
+      </c>
+      <c r="AB330">
+        <v>0</v>
+      </c>
+      <c r="AC330">
+        <v>0</v>
+      </c>
+      <c r="AD330">
+        <v>0</v>
+      </c>
+      <c r="AE330">
+        <v>1</v>
+      </c>
+      <c r="AF330">
+        <v>0</v>
+      </c>
+      <c r="AG330">
+        <v>0</v>
+      </c>
+      <c r="AH330">
+        <v>0</v>
+      </c>
+      <c r="AI330">
+        <v>0</v>
+      </c>
+      <c r="AJ330">
+        <v>0</v>
+      </c>
+      <c r="AK330">
+        <v>1</v>
+      </c>
+      <c r="AL330">
+        <v>0</v>
+      </c>
+      <c r="AM330">
+        <v>0</v>
+      </c>
+      <c r="AN330">
+        <v>0</v>
+      </c>
+      <c r="AO330">
+        <v>0</v>
+      </c>
+      <c r="AP330" t="str">
+        <f t="shared" si="20"/>
+        <v>Winterschläfer</v>
+      </c>
+      <c r="AQ330" t="str">
+        <f t="shared" si="21"/>
+        <v>Winterschläfer</v>
+      </c>
+      <c r="AR330" t="str">
+        <f t="shared" si="22"/>
+        <v>winters97äfer</v>
+      </c>
+      <c r="AS330" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AT330" t="str">
+        <f t="shared" si="24"/>
+        <v>winters97afer</v>
+      </c>
+    </row>
+    <row r="331" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B331">
+        <v>60780</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D331" s="4" t="s">
+        <v>1493</v>
+      </c>
+      <c r="E331" s="4" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F331" s="4">
+        <v>1998</v>
+      </c>
+      <c r="G331">
+        <v>1998</v>
+      </c>
+      <c r="H331">
+        <v>6.3</v>
+      </c>
+      <c r="I331">
+        <v>98</v>
+      </c>
+      <c r="J331">
+        <v>5140</v>
+      </c>
+      <c r="K331" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="L331">
+        <v>-1</v>
+      </c>
+      <c r="M331">
+        <v>26754</v>
+      </c>
+      <c r="N331" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="O331" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="P331" s="1" t="s">
+        <v>1370</v>
+      </c>
+      <c r="Q331">
+        <v>0</v>
+      </c>
+      <c r="R331">
+        <v>0</v>
+      </c>
+      <c r="S331">
+        <v>0</v>
+      </c>
+      <c r="T331">
+        <v>0</v>
+      </c>
+      <c r="U331">
+        <v>0</v>
+      </c>
+      <c r="V331">
+        <v>0</v>
+      </c>
+      <c r="W331">
+        <v>0</v>
+      </c>
+      <c r="X331">
+        <v>0</v>
+      </c>
+      <c r="Y331">
+        <v>0</v>
+      </c>
+      <c r="Z331">
+        <v>0</v>
+      </c>
+      <c r="AA331">
+        <v>0</v>
+      </c>
+      <c r="AB331">
+        <v>0</v>
+      </c>
+      <c r="AC331">
+        <v>1</v>
+      </c>
+      <c r="AD331">
+        <v>1</v>
+      </c>
+      <c r="AE331">
+        <v>1</v>
+      </c>
+      <c r="AF331">
+        <v>0</v>
+      </c>
+      <c r="AG331">
+        <v>0</v>
+      </c>
+      <c r="AH331">
+        <v>0</v>
+      </c>
+      <c r="AI331">
+        <v>0</v>
+      </c>
+      <c r="AJ331">
+        <v>0</v>
+      </c>
+      <c r="AK331">
+        <v>1</v>
+      </c>
+      <c r="AL331">
+        <v>0</v>
+      </c>
+      <c r="AM331">
+        <v>0</v>
+      </c>
+      <c r="AN331">
+        <v>0</v>
+      </c>
+      <c r="AO331">
+        <v>0</v>
+      </c>
+      <c r="AP331" t="str">
+        <f t="shared" si="20"/>
+        <v>The Wisdom of Crocodiles</v>
+      </c>
+      <c r="AQ331" t="str">
+        <f t="shared" si="21"/>
+        <v>Wisdom of Crocodiles</v>
+      </c>
+      <c r="AR331" t="str">
+        <f t="shared" si="22"/>
+        <v>wisdomo98iles</v>
+      </c>
+      <c r="AS331" t="s">
+        <v>1491</v>
+      </c>
+      <c r="AT331" t="str">
+        <f t="shared" si="24"/>
+        <v>wisdom98iles</v>
+      </c>
+    </row>
+    <row r="332" spans="1:46" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B332">
+        <v>1086527</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D332" s="4" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E332" s="4" t="s">
+        <v>1496</v>
+      </c>
+      <c r="F332" s="4">
+        <v>1998</v>
+      </c>
+      <c r="G332">
+        <v>1998</v>
+      </c>
+      <c r="H332">
+        <v>6.1</v>
+      </c>
+      <c r="I332">
+        <v>82</v>
+      </c>
+      <c r="J332">
+        <v>656</v>
+      </c>
+      <c r="K332" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="L332">
+        <v>-1</v>
+      </c>
+      <c r="M332">
+        <v>11057</v>
+      </c>
+      <c r="N332" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="O332" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="Q332">
+        <v>0</v>
+      </c>
+      <c r="R332">
+        <v>0</v>
+      </c>
+      <c r="S332">
+        <v>1</v>
+      </c>
+      <c r="T332">
+        <v>0</v>
+      </c>
+      <c r="U332">
+        <v>0</v>
+      </c>
+      <c r="V332">
+        <v>0</v>
+      </c>
+      <c r="W332">
+        <v>0</v>
+      </c>
+      <c r="X332">
+        <v>0</v>
+      </c>
+      <c r="Y332">
+        <v>0</v>
+      </c>
+      <c r="Z332">
+        <v>0</v>
+      </c>
+      <c r="AA332">
+        <v>0</v>
+      </c>
+      <c r="AB332">
+        <v>0</v>
+      </c>
+      <c r="AC332">
+        <v>0</v>
+      </c>
+      <c r="AD332">
+        <v>0</v>
+      </c>
+      <c r="AE332">
+        <v>0</v>
+      </c>
+      <c r="AF332">
+        <v>0</v>
+      </c>
+      <c r="AG332">
+        <v>0</v>
+      </c>
+      <c r="AH332">
+        <v>0</v>
+      </c>
+      <c r="AI332">
+        <v>0</v>
+      </c>
+      <c r="AJ332">
+        <v>1</v>
+      </c>
+      <c r="AK332">
+        <v>1</v>
+      </c>
+      <c r="AL332">
+        <v>0</v>
+      </c>
+      <c r="AM332">
+        <v>0</v>
+      </c>
+      <c r="AN332">
+        <v>0</v>
+      </c>
+      <c r="AO332">
+        <v>1</v>
+      </c>
+      <c r="AP332" t="str">
+        <f t="shared" si="20"/>
+        <v>The Wolves of Kromer</v>
+      </c>
+      <c r="AQ332" t="str">
+        <f t="shared" si="21"/>
+        <v>Wolves of Kromer</v>
+      </c>
+      <c r="AR332" t="str">
+        <f t="shared" si="22"/>
+        <v>wolveso98omer</v>
+      </c>
+      <c r="AS332" t="s">
+        <v>1494</v>
+      </c>
+      <c r="AT332" t="str">
+        <f t="shared" si="24"/>
+        <v>wolveso98omer</v>
+      </c>
+    </row>
+    <row r="333" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B333">
+        <v>989554</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D333" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="E333" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="F333" s="4">
+        <v>1999</v>
+      </c>
+      <c r="G333">
+        <v>1999</v>
+      </c>
+      <c r="H333">
+        <v>7.2</v>
+      </c>
+      <c r="I333">
+        <v>90</v>
+      </c>
+      <c r="J333">
+        <v>537</v>
+      </c>
+      <c r="K333" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="L333">
+        <v>1200000</v>
+      </c>
+      <c r="M333">
+        <v>110720</v>
+      </c>
+      <c r="N333" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="O333" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="Q333">
+        <v>0</v>
+      </c>
+      <c r="R333">
+        <v>0</v>
+      </c>
+      <c r="S333">
+        <v>0</v>
+      </c>
+      <c r="T333">
+        <v>0</v>
+      </c>
+      <c r="U333">
+        <v>0</v>
+      </c>
+      <c r="V333">
+        <v>0</v>
+      </c>
+      <c r="W333">
+        <v>0</v>
+      </c>
+      <c r="X333">
+        <v>0</v>
+      </c>
+      <c r="Y333">
+        <v>0</v>
+      </c>
+      <c r="Z333">
+        <v>0</v>
+      </c>
+      <c r="AA333">
+        <v>0</v>
+      </c>
+      <c r="AB333">
+        <v>0</v>
+      </c>
+      <c r="AC333">
+        <v>0</v>
+      </c>
+      <c r="AD333">
+        <v>0</v>
+      </c>
+      <c r="AE333">
+        <v>0</v>
+      </c>
+      <c r="AF333">
+        <v>0</v>
+      </c>
+      <c r="AG333">
+        <v>0</v>
+      </c>
+      <c r="AH333">
+        <v>0</v>
+      </c>
+      <c r="AI333">
+        <v>0</v>
+      </c>
+      <c r="AJ333">
+        <v>1</v>
+      </c>
+      <c r="AK333">
+        <v>0</v>
+      </c>
+      <c r="AL333">
+        <v>0</v>
+      </c>
+      <c r="AM333">
+        <v>0</v>
+      </c>
+      <c r="AN333">
+        <v>0</v>
+      </c>
+      <c r="AO333">
+        <v>0</v>
+      </c>
+      <c r="AP333" t="str">
+        <f t="shared" si="20"/>
+        <v>The Woman Chaser</v>
+      </c>
+      <c r="AQ333" t="str">
+        <f t="shared" si="21"/>
+        <v>Woman Chaser</v>
+      </c>
+      <c r="AR333" t="str">
+        <f t="shared" si="22"/>
+        <v>womanch99aser</v>
+      </c>
+      <c r="AS333" t="s">
+        <v>1497</v>
+      </c>
+      <c r="AT333" t="str">
+        <f t="shared" si="24"/>
+        <v>womanch99aser</v>
+      </c>
+    </row>
+    <row r="334" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B334">
+        <v>496107</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D334" s="4" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E334" s="4" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F334" s="4">
+        <v>1999</v>
+      </c>
+      <c r="G334">
+        <v>1999</v>
+      </c>
+      <c r="H334">
+        <v>7.2</v>
+      </c>
+      <c r="I334">
+        <v>108</v>
+      </c>
+      <c r="J334">
+        <v>3643</v>
+      </c>
+      <c r="K334" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="L334">
+        <v>-1</v>
+      </c>
+      <c r="M334">
+        <v>413595</v>
+      </c>
+      <c r="N334" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="O334" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="P334" s="1" t="s">
+        <v>1370</v>
+      </c>
+      <c r="Q334">
+        <v>0</v>
+      </c>
+      <c r="R334">
+        <v>0</v>
+      </c>
+      <c r="S334">
+        <v>0</v>
+      </c>
+      <c r="T334">
+        <v>0</v>
+      </c>
+      <c r="U334">
+        <v>0</v>
+      </c>
+      <c r="V334">
+        <v>0</v>
+      </c>
+      <c r="W334">
+        <v>0</v>
+      </c>
+      <c r="X334">
+        <v>0</v>
+      </c>
+      <c r="Y334">
+        <v>1</v>
+      </c>
+      <c r="Z334">
+        <v>0</v>
+      </c>
+      <c r="AA334">
+        <v>0</v>
+      </c>
+      <c r="AB334">
+        <v>0</v>
+      </c>
+      <c r="AC334">
+        <v>0</v>
+      </c>
+      <c r="AD334">
+        <v>0</v>
+      </c>
+      <c r="AE334">
+        <v>0</v>
+      </c>
+      <c r="AF334">
+        <v>0</v>
+      </c>
+      <c r="AG334">
+        <v>0</v>
+      </c>
+      <c r="AH334">
+        <v>0</v>
+      </c>
+      <c r="AI334">
+        <v>0</v>
+      </c>
+      <c r="AJ334">
+        <v>0</v>
+      </c>
+      <c r="AK334">
+        <v>0</v>
+      </c>
+      <c r="AL334">
+        <v>0</v>
+      </c>
+      <c r="AM334">
+        <v>0</v>
+      </c>
+      <c r="AN334">
+        <v>0</v>
+      </c>
+      <c r="AO334">
+        <v>0</v>
+      </c>
+      <c r="AP334" t="str">
+        <f t="shared" si="20"/>
+        <v>Wonderland</v>
+      </c>
+      <c r="AQ334" t="str">
+        <f t="shared" si="21"/>
+        <v>Wonderland</v>
+      </c>
+      <c r="AR334" t="str">
+        <f t="shared" si="22"/>
+        <v>wonderl99land</v>
+      </c>
+      <c r="AS334" t="s">
+        <v>1501</v>
+      </c>
+      <c r="AT334" t="str">
+        <f t="shared" si="24"/>
+        <v>wonderl99land</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished initial cross-match (yay!)
</commit_message>
<xml_diff>
--- a/data_2017_5_9/imdb/imdb_matches_wf.xlsx
+++ b/data_2017_5_9/imdb/imdb_matches_wf.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\movies\data_2017_5_9\imdb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sciserver\Documents\GitHub\movies\data_2017_5_9\imdb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="imdb_movies1" localSheetId="0">Sheet1!$C$1:$AM$1</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="1504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="1514">
   <si>
     <t>mauvais99ions</t>
   </si>
@@ -4807,6 +4807,36 @@
   </si>
   <si>
     <t>Wonderland</t>
+  </si>
+  <si>
+    <t>ekkusu96kusu</t>
+  </si>
+  <si>
+    <t>Ekkusu (1996)</t>
+  </si>
+  <si>
+    <t>Ekkusu</t>
+  </si>
+  <si>
+    <t>younggi99soon</t>
+  </si>
+  <si>
+    <t>The Young Girl and the Monsoon (1999)</t>
+  </si>
+  <si>
+    <t>The Young Girl and the Monsoon</t>
+  </si>
+  <si>
+    <t>0000111111</t>
+  </si>
+  <si>
+    <t>zhenghu98ishi</t>
+  </si>
+  <si>
+    <t>Zheng hun qi shi (1998)</t>
+  </si>
+  <si>
+    <t>Zheng hun qi shi</t>
   </si>
 </sst>
 </file>
@@ -5205,10 +5235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT334"/>
+  <dimension ref="A1:AT337"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="A334" sqref="A334"/>
+      <selection activeCell="E334" sqref="E334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -44178,15 +44208,15 @@
         <v>0</v>
       </c>
       <c r="AP281" t="str">
-        <f t="shared" ref="AP281:AP334" si="20">IF(LEFT(D281,2)="A",MID(D281,3,9999),D281)</f>
+        <f t="shared" ref="AP281:AP337" si="20">IF(LEFT(D281,2)="A",MID(D281,3,9999),D281)</f>
         <v>Swiri</v>
       </c>
       <c r="AQ281" t="str">
-        <f t="shared" ref="AQ281:AQ334" si="21">IF(LEFT(AP281,4)="The ",MID(AP281,5,9999),AP281)</f>
+        <f t="shared" ref="AQ281:AQ337" si="21">IF(LEFT(AP281,4)="The ",MID(AP281,5,9999),AP281)</f>
         <v>Swiri</v>
       </c>
       <c r="AR281" t="str">
-        <f t="shared" ref="AR281:AR334" si="22">LOWER(CONCATENATE(LEFT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),7),RIGHT(F281,2),RIGHT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),4)))</f>
+        <f t="shared" ref="AR281:AR337" si="22">LOWER(CONCATENATE(LEFT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),7),RIGHT(F281,2),RIGHT(SUBSTITUTE(TRIM(CLEAN(AQ281))," ",""),4)))</f>
         <v>swiri99wiri</v>
       </c>
       <c r="AS281" t="str">
@@ -50889,7 +50919,7 @@
         <v>1485</v>
       </c>
       <c r="AT329" t="str">
-        <f t="shared" ref="AT329:AT334" si="24">IF(ISBLANK(AS329),AR329,AS329)</f>
+        <f t="shared" ref="AT329:AT337" si="24">IF(ISBLANK(AS329),AR329,AS329)</f>
         <v>badmara99bord</v>
       </c>
     </row>
@@ -51602,6 +51632,432 @@
       <c r="AT334" t="str">
         <f t="shared" si="24"/>
         <v>wonderl99land</v>
+      </c>
+    </row>
+    <row r="335" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B335">
+        <v>903734</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D335" s="4" t="s">
+        <v>1506</v>
+      </c>
+      <c r="E335" s="4" t="s">
+        <v>1506</v>
+      </c>
+      <c r="F335" s="4">
+        <v>1996</v>
+      </c>
+      <c r="G335">
+        <v>1996</v>
+      </c>
+      <c r="H335">
+        <v>6.2</v>
+      </c>
+      <c r="I335">
+        <v>100</v>
+      </c>
+      <c r="J335">
+        <v>2190</v>
+      </c>
+      <c r="K335" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="L335">
+        <v>-1</v>
+      </c>
+      <c r="M335">
+        <v>160113</v>
+      </c>
+      <c r="N335" s="1" t="s">
+        <v>1336</v>
+      </c>
+      <c r="O335" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="P335" s="1" t="s">
+        <v>1370</v>
+      </c>
+      <c r="Q335">
+        <v>0</v>
+      </c>
+      <c r="R335">
+        <v>0</v>
+      </c>
+      <c r="S335">
+        <v>1</v>
+      </c>
+      <c r="T335">
+        <v>0</v>
+      </c>
+      <c r="U335">
+        <v>0</v>
+      </c>
+      <c r="V335">
+        <v>0</v>
+      </c>
+      <c r="W335">
+        <v>0</v>
+      </c>
+      <c r="X335">
+        <v>0</v>
+      </c>
+      <c r="Y335">
+        <v>0</v>
+      </c>
+      <c r="Z335">
+        <v>1</v>
+      </c>
+      <c r="AA335">
+        <v>0</v>
+      </c>
+      <c r="AB335">
+        <v>0</v>
+      </c>
+      <c r="AC335">
+        <v>0</v>
+      </c>
+      <c r="AD335">
+        <v>0</v>
+      </c>
+      <c r="AE335">
+        <v>1</v>
+      </c>
+      <c r="AF335">
+        <v>0</v>
+      </c>
+      <c r="AG335">
+        <v>0</v>
+      </c>
+      <c r="AH335">
+        <v>1</v>
+      </c>
+      <c r="AI335">
+        <v>0</v>
+      </c>
+      <c r="AJ335">
+        <v>0</v>
+      </c>
+      <c r="AK335">
+        <v>0</v>
+      </c>
+      <c r="AL335">
+        <v>0</v>
+      </c>
+      <c r="AM335">
+        <v>0</v>
+      </c>
+      <c r="AN335">
+        <v>0</v>
+      </c>
+      <c r="AO335">
+        <v>1</v>
+      </c>
+      <c r="AP335" t="str">
+        <f t="shared" si="20"/>
+        <v>Ekkusu</v>
+      </c>
+      <c r="AQ335" t="str">
+        <f t="shared" si="21"/>
+        <v>Ekkusu</v>
+      </c>
+      <c r="AR335" t="str">
+        <f t="shared" si="22"/>
+        <v>ekkusu96kusu</v>
+      </c>
+      <c r="AS335" t="s">
+        <v>1504</v>
+      </c>
+      <c r="AT335" t="str">
+        <f t="shared" si="24"/>
+        <v>ekkusu96kusu</v>
+      </c>
+    </row>
+    <row r="336" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B336">
+        <v>983026</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D336" s="4" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E336" s="4" t="s">
+        <v>1509</v>
+      </c>
+      <c r="F336" s="4">
+        <v>1999</v>
+      </c>
+      <c r="G336">
+        <v>1999</v>
+      </c>
+      <c r="H336">
+        <v>5.2</v>
+      </c>
+      <c r="I336">
+        <v>90</v>
+      </c>
+      <c r="J336">
+        <v>110</v>
+      </c>
+      <c r="K336" s="1" t="s">
+        <v>1510</v>
+      </c>
+      <c r="L336">
+        <v>-1</v>
+      </c>
+      <c r="M336">
+        <v>8759</v>
+      </c>
+      <c r="N336" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="O336" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="Q336">
+        <v>0</v>
+      </c>
+      <c r="R336">
+        <v>0</v>
+      </c>
+      <c r="S336">
+        <v>0</v>
+      </c>
+      <c r="T336">
+        <v>0</v>
+      </c>
+      <c r="U336">
+        <v>0</v>
+      </c>
+      <c r="V336">
+        <v>0</v>
+      </c>
+      <c r="W336">
+        <v>0</v>
+      </c>
+      <c r="X336">
+        <v>0</v>
+      </c>
+      <c r="Y336">
+        <v>0</v>
+      </c>
+      <c r="Z336">
+        <v>0</v>
+      </c>
+      <c r="AA336">
+        <v>0</v>
+      </c>
+      <c r="AB336">
+        <v>0</v>
+      </c>
+      <c r="AC336">
+        <v>0</v>
+      </c>
+      <c r="AD336">
+        <v>0</v>
+      </c>
+      <c r="AE336">
+        <v>0</v>
+      </c>
+      <c r="AF336">
+        <v>0</v>
+      </c>
+      <c r="AG336">
+        <v>0</v>
+      </c>
+      <c r="AH336">
+        <v>0</v>
+      </c>
+      <c r="AI336">
+        <v>0</v>
+      </c>
+      <c r="AJ336">
+        <v>1</v>
+      </c>
+      <c r="AK336">
+        <v>0</v>
+      </c>
+      <c r="AL336">
+        <v>0</v>
+      </c>
+      <c r="AM336">
+        <v>0</v>
+      </c>
+      <c r="AN336">
+        <v>0</v>
+      </c>
+      <c r="AO336">
+        <v>0</v>
+      </c>
+      <c r="AP336" t="str">
+        <f t="shared" si="20"/>
+        <v>The Young Girl and the Monsoon</v>
+      </c>
+      <c r="AQ336" t="str">
+        <f t="shared" si="21"/>
+        <v>Young Girl and the Monsoon</v>
+      </c>
+      <c r="AR336" t="str">
+        <f t="shared" si="22"/>
+        <v>younggi99soon</v>
+      </c>
+      <c r="AS336" t="s">
+        <v>1507</v>
+      </c>
+      <c r="AT336" t="str">
+        <f t="shared" si="24"/>
+        <v>younggi99soon</v>
+      </c>
+    </row>
+    <row r="337" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B337">
+        <v>190520</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D337" s="4" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E337" s="4" t="s">
+        <v>1513</v>
+      </c>
+      <c r="F337" s="4">
+        <v>1998</v>
+      </c>
+      <c r="G337">
+        <v>1998</v>
+      </c>
+      <c r="H337">
+        <v>7.2</v>
+      </c>
+      <c r="I337">
+        <v>96</v>
+      </c>
+      <c r="J337">
+        <v>453</v>
+      </c>
+      <c r="K337" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="L337">
+        <v>-1</v>
+      </c>
+      <c r="M337">
+        <v>20267</v>
+      </c>
+      <c r="N337" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="O337" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="Q337">
+        <v>0</v>
+      </c>
+      <c r="R337">
+        <v>0</v>
+      </c>
+      <c r="S337">
+        <v>0</v>
+      </c>
+      <c r="T337">
+        <v>0</v>
+      </c>
+      <c r="U337">
+        <v>0</v>
+      </c>
+      <c r="V337">
+        <v>0</v>
+      </c>
+      <c r="W337">
+        <v>0</v>
+      </c>
+      <c r="X337">
+        <v>0</v>
+      </c>
+      <c r="Y337">
+        <v>1</v>
+      </c>
+      <c r="Z337">
+        <v>0</v>
+      </c>
+      <c r="AA337">
+        <v>0</v>
+      </c>
+      <c r="AB337">
+        <v>0</v>
+      </c>
+      <c r="AC337">
+        <v>0</v>
+      </c>
+      <c r="AD337">
+        <v>0</v>
+      </c>
+      <c r="AE337">
+        <v>0</v>
+      </c>
+      <c r="AF337">
+        <v>0</v>
+      </c>
+      <c r="AG337">
+        <v>0</v>
+      </c>
+      <c r="AH337">
+        <v>0</v>
+      </c>
+      <c r="AI337">
+        <v>0</v>
+      </c>
+      <c r="AJ337">
+        <v>1</v>
+      </c>
+      <c r="AK337">
+        <v>1</v>
+      </c>
+      <c r="AL337">
+        <v>0</v>
+      </c>
+      <c r="AM337">
+        <v>0</v>
+      </c>
+      <c r="AN337">
+        <v>0</v>
+      </c>
+      <c r="AO337">
+        <v>0</v>
+      </c>
+      <c r="AP337" t="str">
+        <f t="shared" si="20"/>
+        <v>Zheng hun qi shi</v>
+      </c>
+      <c r="AQ337" t="str">
+        <f t="shared" si="21"/>
+        <v>Zheng hun qi shi</v>
+      </c>
+      <c r="AR337" t="str">
+        <f t="shared" si="22"/>
+        <v>zhenghu98ishi</v>
+      </c>
+      <c r="AS337" t="s">
+        <v>1511</v>
+      </c>
+      <c r="AT337" t="str">
+        <f t="shared" si="24"/>
+        <v>zhenghu98ishi</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished scripts for May 2017 dataset
The craptop version of the scripts only
</commit_message>
<xml_diff>
--- a/data_2017_5_9/imdb/imdb_matches_wf.xlsx
+++ b/data_2017_5_9/imdb/imdb_matches_wf.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="1514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="1514">
   <si>
     <t>mauvais99ions</t>
   </si>
@@ -4761,18 +4761,12 @@
     <t>Bad ma ra khahad bord</t>
   </si>
   <si>
-    <t>winters97afer</t>
-  </si>
-  <si>
     <t>Winterschläfer (1997)</t>
   </si>
   <si>
     <t>Winterschläfer</t>
   </si>
   <si>
-    <t>wisdom98iles</t>
-  </si>
-  <si>
     <t>The Wisdom of Crocodiles (1998)</t>
   </si>
   <si>
@@ -4837,6 +4831,12 @@
   </si>
   <si>
     <t>Zheng hun qi shi</t>
+  </si>
+  <si>
+    <t>winters97äfer</t>
+  </si>
+  <si>
+    <t>wisdomo98iles</t>
   </si>
 </sst>
 </file>
@@ -5237,9 +5237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="E334" sqref="E334"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -49938,7 +49936,7 @@
         <v>wadd:th99lmes</v>
       </c>
       <c r="AS322" t="str">
-        <f t="shared" ref="AS322:AS328" si="23">IF(ISBLANK(AR322),AQ322,AR322)</f>
+        <f t="shared" ref="AS322:AS337" si="23">IF(ISBLANK(AR322),AQ322,AR322)</f>
         <v>wadd:th99lmes</v>
       </c>
     </row>
@@ -50915,8 +50913,9 @@
         <f t="shared" si="22"/>
         <v>badmara99bord</v>
       </c>
-      <c r="AS329" t="s">
-        <v>1485</v>
+      <c r="AS329" t="str">
+        <f t="shared" si="23"/>
+        <v>badmara99bord</v>
       </c>
       <c r="AT329" t="str">
         <f t="shared" ref="AT329:AT337" si="24">IF(ISBLANK(AS329),AR329,AS329)</f>
@@ -50925,19 +50924,19 @@
     </row>
     <row r="330" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>1488</v>
+        <v>1512</v>
       </c>
       <c r="B330">
         <v>353254</v>
       </c>
       <c r="C330" s="1" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D330" s="4" t="s">
         <v>1489</v>
       </c>
-      <c r="D330" s="4" t="s">
-        <v>1490</v>
-      </c>
       <c r="E330" s="4" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="F330" s="4">
         <v>1997</v>
@@ -51056,29 +51055,30 @@
         <f t="shared" si="22"/>
         <v>winters97äfer</v>
       </c>
-      <c r="AS330" t="s">
-        <v>1488</v>
+      <c r="AS330" t="str">
+        <f t="shared" si="23"/>
+        <v>winters97äfer</v>
       </c>
       <c r="AT330" t="str">
         <f t="shared" si="24"/>
-        <v>winters97afer</v>
+        <v>winters97äfer</v>
       </c>
     </row>
     <row r="331" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>1491</v>
+        <v>1513</v>
       </c>
       <c r="B331">
         <v>60780</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="D331" s="4" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="E331" s="4" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="F331" s="4">
         <v>1998</v>
@@ -51200,29 +51200,30 @@
         <f t="shared" si="22"/>
         <v>wisdomo98iles</v>
       </c>
-      <c r="AS331" t="s">
-        <v>1491</v>
+      <c r="AS331" t="str">
+        <f t="shared" si="23"/>
+        <v>wisdomo98iles</v>
       </c>
       <c r="AT331" t="str">
         <f t="shared" si="24"/>
-        <v>wisdom98iles</v>
+        <v>wisdomo98iles</v>
       </c>
     </row>
     <row r="332" spans="1:46" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="B332">
         <v>1086527</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="D332" s="4" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="E332" s="4" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="F332" s="4">
         <v>1998</v>
@@ -51341,8 +51342,9 @@
         <f t="shared" si="22"/>
         <v>wolveso98omer</v>
       </c>
-      <c r="AS332" t="s">
-        <v>1494</v>
+      <c r="AS332" t="str">
+        <f t="shared" si="23"/>
+        <v>wolveso98omer</v>
       </c>
       <c r="AT332" t="str">
         <f t="shared" si="24"/>
@@ -51351,19 +51353,19 @@
     </row>
     <row r="333" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="B333">
         <v>989554</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="D333" s="4" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="E333" s="4" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="F333" s="4">
         <v>1999</v>
@@ -51381,7 +51383,7 @@
         <v>537</v>
       </c>
       <c r="K333" s="1" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="L333">
         <v>1200000</v>
@@ -51482,8 +51484,9 @@
         <f t="shared" si="22"/>
         <v>womanch99aser</v>
       </c>
-      <c r="AS333" t="s">
-        <v>1497</v>
+      <c r="AS333" t="str">
+        <f t="shared" si="23"/>
+        <v>womanch99aser</v>
       </c>
       <c r="AT333" t="str">
         <f t="shared" si="24"/>
@@ -51492,19 +51495,19 @@
     </row>
     <row r="334" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="B334">
         <v>496107</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="D334" s="4" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="E334" s="4" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="F334" s="4">
         <v>1999</v>
@@ -51626,8 +51629,9 @@
         <f t="shared" si="22"/>
         <v>wonderl99land</v>
       </c>
-      <c r="AS334" t="s">
-        <v>1501</v>
+      <c r="AS334" t="str">
+        <f t="shared" si="23"/>
+        <v>wonderl99land</v>
       </c>
       <c r="AT334" t="str">
         <f t="shared" si="24"/>
@@ -51636,19 +51640,19 @@
     </row>
     <row r="335" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="B335">
         <v>903734</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="D335" s="4" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="E335" s="4" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="F335" s="4">
         <v>1996</v>
@@ -51770,8 +51774,9 @@
         <f t="shared" si="22"/>
         <v>ekkusu96kusu</v>
       </c>
-      <c r="AS335" t="s">
-        <v>1504</v>
+      <c r="AS335" t="str">
+        <f t="shared" si="23"/>
+        <v>ekkusu96kusu</v>
       </c>
       <c r="AT335" t="str">
         <f t="shared" si="24"/>
@@ -51780,19 +51785,19 @@
     </row>
     <row r="336" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="B336">
         <v>983026</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="D336" s="4" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="E336" s="4" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="F336" s="4">
         <v>1999</v>
@@ -51810,7 +51815,7 @@
         <v>110</v>
       </c>
       <c r="K336" s="1" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="L336">
         <v>-1</v>
@@ -51911,8 +51916,9 @@
         <f t="shared" si="22"/>
         <v>younggi99soon</v>
       </c>
-      <c r="AS336" t="s">
-        <v>1507</v>
+      <c r="AS336" t="str">
+        <f t="shared" si="23"/>
+        <v>younggi99soon</v>
       </c>
       <c r="AT336" t="str">
         <f t="shared" si="24"/>
@@ -51921,19 +51927,19 @@
     </row>
     <row r="337" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="B337">
         <v>190520</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="D337" s="4" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="E337" s="4" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="F337" s="4">
         <v>1998</v>
@@ -52052,8 +52058,9 @@
         <f t="shared" si="22"/>
         <v>zhenghu98ishi</v>
       </c>
-      <c r="AS337" t="s">
-        <v>1511</v>
+      <c r="AS337" t="str">
+        <f t="shared" si="23"/>
+        <v>zhenghu98ishi</v>
       </c>
       <c r="AT337" t="str">
         <f t="shared" si="24"/>

</xml_diff>